<commit_message>
Converted data to CSV
</commit_message>
<xml_diff>
--- a/data/policeforceareadatatablesyearendingjune13_tcm77-330992.xlsx
+++ b/data/policeforceareadatatablesyearendingjune13_tcm77-330992.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015"/>
+    <workbookView xWindow="120" yWindow="20" windowWidth="19040" windowHeight="12020"/>
   </bookViews>
   <sheets>
-    <sheet name="Table P1" sheetId="7" r:id="rId1"/>
+    <sheet name="policeforceareadatatablesyearen" sheetId="7" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="ForceNames">'[1]Apr-Jun 2011'!$A$5:$A$47</definedName>
     <definedName name="owners">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Table P1'!$A$1:$AA$78</definedName>
-    <definedName name="Table">OFFSET([3]tbl_NATIONAL!$A$2,0,0,COUNTA([3]tbl_NATIONAL!XFD$1:XFD$65536)-1,14)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">policeforceareadatatablesyearen!$A$1:$AA$78</definedName>
+    <definedName name="Table">OFFSET([2]tbl_NATIONAL!$A$2,0,0,COUNTA([2]tbl_NATIONAL!XFD$1:XFD$65536)-1,14)</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -335,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +461,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -484,7 +496,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -494,7 +506,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,15 +514,15 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,6 +560,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -699,9 +712,10 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="Comma 2" xfId="1"/>
     <cellStyle name="Comma 3" xfId="2"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
     <cellStyle name="Hyperlink 2 2" xfId="4"/>
     <cellStyle name="Hyperlink 3" xfId="5"/>
@@ -731,7 +745,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Annual confirmation"/>
@@ -986,22 +1000,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Incident rate"/>
-      <sheetName val="Prevelance rate"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Population multipliers"/>
@@ -1312,36 +1311,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="8" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="8" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" style="8" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" style="30" customWidth="1"/>
-    <col min="9" max="12" width="9.7109375" style="8" customWidth="1"/>
-    <col min="13" max="14" width="9.7109375" style="30" customWidth="1"/>
-    <col min="15" max="20" width="9.7109375" style="8" customWidth="1"/>
-    <col min="21" max="21" width="4.28515625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="8" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="8" customWidth="1"/>
-    <col min="24" max="24" width="9.7109375" style="8" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="8" customWidth="1"/>
-    <col min="26" max="26" width="4.28515625" style="8" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" style="8" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="27.6640625" style="8" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" style="8" customWidth="1"/>
+    <col min="7" max="8" width="9.6640625" style="30" customWidth="1"/>
+    <col min="9" max="12" width="9.6640625" style="8" customWidth="1"/>
+    <col min="13" max="14" width="9.6640625" style="30" customWidth="1"/>
+    <col min="15" max="20" width="9.6640625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="4.33203125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" style="8" customWidth="1"/>
+    <col min="24" max="24" width="9.6640625" style="8" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="8" customWidth="1"/>
+    <col min="26" max="26" width="4.33203125" style="8" customWidth="1"/>
+    <col min="27" max="27" width="9.6640625" style="8" customWidth="1"/>
+    <col min="28" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>86</v>
       </c>
@@ -1372,7 +1371,7 @@
       <c r="Z1" s="42"/>
       <c r="AA1" s="42"/>
     </row>
-    <row r="2" spans="1:27" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="3" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1398,7 +1397,7 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -1425,7 +1424,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="43" t="s">
         <v>83</v>
@@ -1462,7 +1461,7 @@
       <c r="Z4" s="40"/>
       <c r="AA4" s="40"/>
     </row>
-    <row r="5" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="60" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -1533,7 +1532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13.5" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="41" t="s">
         <v>81</v>
@@ -1563,7 +1562,7 @@
       <c r="Y6" s="41"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="12" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>3</v>
       </c>
@@ -1794,7 +1793,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="12" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="20"/>
@@ -1899,7 +1898,7 @@
       <c r="Z11" s="25"/>
       <c r="AA11" s="21"/>
     </row>
-    <row r="12" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="12" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1976,7 +1975,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="12" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="12" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -2130,7 +2129,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="12" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="12" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2283,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="22" t="s">
         <v>10</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>7572</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="12" customHeight="1">
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="20"/>
@@ -2389,7 +2388,7 @@
       <c r="Z18" s="25"/>
       <c r="AA18" s="21"/>
     </row>
-    <row r="19" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="12" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>11</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="12" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
@@ -2543,7 +2542,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="12" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="12" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>14</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>3867</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>87</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>7661</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="12" customHeight="1">
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="20"/>
@@ -2802,7 +2801,7 @@
       <c r="Z24" s="25"/>
       <c r="AA24" s="21"/>
     </row>
-    <row r="25" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="12" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
@@ -2879,7 +2878,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="12" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>16</v>
       </c>
@@ -2956,7 +2955,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="12" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="12" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>18</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="12" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>19</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="22" t="s">
         <v>20</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>4165</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="12" customHeight="1">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="20"/>
@@ -3292,7 +3291,7 @@
       <c r="Z31" s="25"/>
       <c r="AA31" s="21"/>
     </row>
-    <row r="32" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="12" customHeight="1">
       <c r="A32" s="8" t="s">
         <v>21</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="12" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>22</v>
       </c>
@@ -3446,7 +3445,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="12" customHeight="1">
       <c r="A34" s="8" t="s">
         <v>23</v>
       </c>
@@ -3523,7 +3522,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="12" customHeight="1">
       <c r="A35" s="8" t="s">
         <v>24</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="36" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A36" s="22" t="s">
         <v>25</v>
       </c>
@@ -3677,7 +3676,7 @@
         <v>7287</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="12" customHeight="1">
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
       <c r="D37" s="20"/>
@@ -3705,7 +3704,7 @@
       <c r="Z37" s="25"/>
       <c r="AA37" s="21"/>
     </row>
-    <row r="38" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="12" customHeight="1">
       <c r="A38" s="8" t="s">
         <v>26</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="12" customHeight="1">
       <c r="A39" s="8" t="s">
         <v>27</v>
       </c>
@@ -3859,7 +3858,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="12" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>28</v>
       </c>
@@ -3936,7 +3935,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="12" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>29</v>
       </c>
@@ -4013,7 +4012,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="12" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>30</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="12" customHeight="1">
       <c r="A43" s="8" t="s">
         <v>31</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A44" s="22" t="s">
         <v>32</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>5990</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" ht="12" customHeight="1">
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="20"/>
@@ -4272,7 +4271,7 @@
       <c r="Z45" s="25"/>
       <c r="AA45" s="21"/>
     </row>
-    <row r="46" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" ht="12" customHeight="1">
       <c r="A46" s="8" t="s">
         <v>33</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="12" customHeight="1">
       <c r="A47" s="8" t="s">
         <v>34</v>
       </c>
@@ -4426,7 +4425,7 @@
         <v>26756</v>
       </c>
     </row>
-    <row r="48" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A48" s="22" t="s">
         <v>35</v>
       </c>
@@ -4503,7 +4502,7 @@
         <v>26786</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="12" customHeight="1">
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
       <c r="D49" s="20"/>
@@ -4531,7 +4530,7 @@
       <c r="Z49" s="25"/>
       <c r="AA49" s="21"/>
     </row>
-    <row r="50" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="12" customHeight="1">
       <c r="A50" s="8" t="s">
         <v>36</v>
       </c>
@@ -4608,7 +4607,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="12" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>37</v>
       </c>
@@ -4685,7 +4684,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="12" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>38</v>
       </c>
@@ -4762,7 +4761,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="12" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>39</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" ht="12" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>40</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>4235</v>
       </c>
     </row>
-    <row r="55" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A55" s="22" t="s">
         <v>41</v>
       </c>
@@ -4993,7 +4992,7 @@
         <v>11268</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" ht="12" customHeight="1">
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
       <c r="D56" s="20"/>
@@ -5021,7 +5020,7 @@
       <c r="Z56" s="25"/>
       <c r="AA56" s="21"/>
     </row>
-    <row r="57" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" ht="12" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>42</v>
       </c>
@@ -5098,7 +5097,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="12" customHeight="1">
       <c r="A58" s="8" t="s">
         <v>43</v>
       </c>
@@ -5175,7 +5174,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="12" customHeight="1">
       <c r="A59" s="8" t="s">
         <v>44</v>
       </c>
@@ -5252,7 +5251,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="12" customHeight="1">
       <c r="A60" s="8" t="s">
         <v>45</v>
       </c>
@@ -5329,7 +5328,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" ht="12" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>46</v>
       </c>
@@ -5406,7 +5405,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="62" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A62" s="22" t="s">
         <v>47</v>
       </c>
@@ -5483,7 +5482,7 @@
         <v>4713</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" ht="12" customHeight="1">
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
       <c r="D63" s="20"/>
@@ -5511,7 +5510,7 @@
       <c r="Z63" s="25"/>
       <c r="AA63" s="21"/>
     </row>
-    <row r="64" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A64" s="22" t="s">
         <v>48</v>
       </c>
@@ -5588,7 +5587,7 @@
         <v>77113</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" ht="12" customHeight="1">
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
       <c r="D65" s="20"/>
@@ -5616,7 +5615,7 @@
       <c r="Z65" s="25"/>
       <c r="AA65" s="21"/>
     </row>
-    <row r="66" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="12" customHeight="1">
       <c r="A66" s="8" t="s">
         <v>49</v>
       </c>
@@ -5693,7 +5692,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" ht="12" customHeight="1">
       <c r="A67" s="8" t="s">
         <v>50</v>
       </c>
@@ -5770,7 +5769,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" ht="12" customHeight="1">
       <c r="A68" s="8" t="s">
         <v>51</v>
       </c>
@@ -5847,7 +5846,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" ht="12" customHeight="1">
       <c r="A69" s="8" t="s">
         <v>52</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="70" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" s="22" customFormat="1" ht="12" customHeight="1">
       <c r="A70" s="22" t="s">
         <v>53</v>
       </c>
@@ -6001,7 +6000,7 @@
         <v>2433</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" ht="12" customHeight="1">
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
       <c r="D71" s="20"/>
@@ -6029,7 +6028,7 @@
       <c r="Z71" s="25"/>
       <c r="AA71" s="21"/>
     </row>
-    <row r="72" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1">
       <c r="A72" s="26" t="s">
         <v>54</v>
       </c>
@@ -6106,7 +6105,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1">
       <c r="A73" s="26"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -6135,7 +6134,7 @@
       <c r="Z73" s="21"/>
       <c r="AA73" s="21"/>
     </row>
-    <row r="74" spans="1:27" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" s="27" customFormat="1" ht="13.5" customHeight="1">
       <c r="A74" s="26" t="s">
         <v>82</v>
       </c>
@@ -6212,7 +6211,7 @@
         <v>150389</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="12" customHeight="1">
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
       <c r="D75" s="20"/>
@@ -6240,7 +6239,7 @@
       <c r="Z75" s="25"/>
       <c r="AA75" s="21"/>
     </row>
-    <row r="76" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1">
       <c r="A76" s="28" t="s">
         <v>56</v>
       </c>
@@ -6317,7 +6316,7 @@
         <v>230335</v>
       </c>
     </row>
-    <row r="77" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" s="27" customFormat="1" ht="12" customHeight="1">
       <c r="A77" s="34" t="s">
         <v>58</v>
       </c>
@@ -6348,7 +6347,7 @@
       <c r="Z77" s="37"/>
       <c r="AA77" s="37"/>
     </row>
-    <row r="78" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="24" customHeight="1">
       <c r="A78" s="38" t="s">
         <v>85</v>
       </c>
@@ -6379,7 +6378,7 @@
       <c r="Z78" s="38"/>
       <c r="AA78" s="38"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27">
       <c r="B79" s="31"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
@@ -6406,19 +6405,24 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A78:AA78"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="E4:T4"/>
-    <mergeCell ref="V4:AA4"/>
-    <mergeCell ref="B6:Y6"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A78:AA78"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B6:Y6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A78" r:id="rId1" display="4. Action Fraud have taken over the recording of fraud offences on behalf of individual police forces. This process began in April 2011 and was rolled out to all police forces by March 2013. Due to this change, caution should be applied when comparing dat"/>
   </hyperlinks>
   <pageMargins left="1.2598425196850394" right="0.27559055118110237" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="8" scale="71" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>